<commit_message>
refactored code and tested if records were updating correctly on excel
</commit_message>
<xml_diff>
--- a/src/database_logic/test-data/users_db.xlsx
+++ b/src/database_logic/test-data/users_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coded\OneDrive\Desktop\loanpro-challenge-aws-lambda-backend\src\databases\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coded\OneDrive\Desktop\loanpro-challenge-aws-lambda-backend\src\database_logic\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9FC7FB-EC10-48EE-A5A9-8DFAF8E447B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4782EABC-D7C4-4325-BFDA-6AEE7016ABF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="2475" windowWidth="18915" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9780" yWindow="1650" windowWidth="27195" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UsersTable" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -36,6 +36,12 @@
     <t>status</t>
   </si>
   <si>
+    <t>last_login</t>
+  </si>
+  <si>
+    <t>flagged</t>
+  </si>
+  <si>
     <t>luissantanderdev@gmail.com</t>
   </si>
   <si>
@@ -45,55 +51,165 @@
     <t>active</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>codedinsound@gmail.com</t>
   </si>
   <si>
     <t>inactive</t>
   </si>
   <si>
+    <t>inactiveaccounttest@gmail.com</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
     <t>user_id</t>
   </si>
   <si>
     <t>balance</t>
   </si>
   <si>
-    <t>records</t>
-  </si>
-  <si>
-    <t>{}</t>
-  </si>
-  <si>
-    <t>inactiveaccounttest@gmail.com</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t>last_login</t>
-  </si>
-  <si>
-    <t>flagged</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>operation_id</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>user_balance</t>
+  </si>
+  <si>
+    <t>operation_response</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>{"status":"balance',_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
+  'updated","date":"2023-01-21T22:08:50.429Z","balance":100600.53}</t>
+  </si>
+  <si>
+    <t>Sat Jan 20 2023 16:18:57 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:28:57.573Z","balance":2000}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:28:57 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>SUBTRACT</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:29:32.572Z","balance":1000}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:29:32 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>MULTIPLY</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:29:57.589Z","balance":3000}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:29:57 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:08.086Z","balance":3004}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:08 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-6</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:09.814Z","balance":3008}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:09 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:11.366Z","balance":3012}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:11 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-8</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:12.630Z","balance":3016}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:12 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-9</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:13.918Z","balance":3020}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:13 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-10</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:15.147Z","balance":3024}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:15 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-11</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:16.389Z","balance":3028}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:16 GMT-0700 (Mountain Standard Time)</t>
+  </si>
+  <si>
+    <t>1-12</t>
+  </si>
+  <si>
+    <t>{"status":"balance-updated","date":"2023-01-21T23:39:17.608Z","balance":3032}</t>
+  </si>
+  <si>
+    <t>Sat Jan 21 2023 16:39:17 GMT-0700 (Mountain Standard Time)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,16 +232,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,13 +554,15 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.875" customWidth="1"/>
-    <col min="3" max="3" width="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.25" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -464,10 +579,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -475,16 +590,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -492,44 +607,44 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{BFF7A634-D01E-450E-BCA4-87AABDAD91ED}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D3 A5:D1961" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -544,10 +659,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -555,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100500.53</v>
+        <v>3032</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -576,40 +691,317 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>3004</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3008</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3012</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>3016</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>3020</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>3024</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>3028</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>3032</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>